<commit_message>
add two other columns
Signed-off-by: Thiago Farina <tfransosi@gmail.com>
</commit_message>
<xml_diff>
--- a/c/apps/moneybin/b3/CLASSIFICACAO-SETORIAL.xlsx
+++ b/c/apps/moneybin/b3/CLASSIFICACAO-SETORIAL.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Setor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsetor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segmento</t>
   </si>
   <si>
     <t xml:space="preserve">Bens Industriais</t>
@@ -151,10 +157,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -167,60 +173,66 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>